<commit_message>
Add Jing Chen's third diary
</commit_message>
<xml_diff>
--- a/diaries/diary-JingChen.xlsx
+++ b/diaries/diary-JingChen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigAnnie\Desktop\winter2020\swe265-reqt\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigAnnie\Desktop\winter2020\swe265-0121\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE3A96-4C51-4B04-AF18-542B5ED287DE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903C64D8-D1D1-443A-84C8-B3891F21FA0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="11136" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Participants</t>
   </si>
   <si>
-    <t>&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what time?&gt;</t>
-  </si>
-  <si>
     <t>Reflection</t>
   </si>
   <si>
@@ -66,30 +60,15 @@
     <t>&lt;your github profile&gt;</t>
   </si>
   <si>
-    <t>&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
     <t>Your Overall Mood</t>
   </si>
   <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
     <t>Achievements</t>
   </si>
   <si>
-    <t>&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
-  </si>
-  <si>
     <t>Etc.</t>
   </si>
   <si>
@@ -130,6 +109,24 @@
   </si>
   <si>
     <t>Dongxin Xiang, Guowei Li</t>
+  </si>
+  <si>
+    <t>17:00-19:00</t>
+  </si>
+  <si>
+    <t>Learn mental model, how to externize mental model using UML</t>
+  </si>
+  <si>
+    <t>I really enjoy practicing and discussing with classmates, every time we can learn from each other. This time when try to find out how scoring is implemented in JPacman3. It was interesting.</t>
+  </si>
+  <si>
+    <t>Enjoyable. But I couldn't generate a UML in class, which made me a little upset, since it is the second time my IntelliJ couldn't work well in class. I hope I can have time to prepare before class, so that I can follow up.</t>
+  </si>
+  <si>
+    <t>Rafael Oliveira; Dongxin Xiang, Guowei Li</t>
+  </si>
+  <si>
+    <t>Know about usage of mental model, and how to improve mental model using UML by practice with examples.. After class, I did homework with my partners, which also help me understand what I have learned in class.</t>
   </si>
 </sst>
 </file>
@@ -309,11 +306,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -636,7 +633,7 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:G12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,24 +642,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
@@ -678,10 +675,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -693,10 +690,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -708,10 +705,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -737,26 +734,26 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>14</v>
+      <c r="D9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="62" x14ac:dyDescent="0.35">
@@ -764,20 +761,20 @@
         <v>43839</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
@@ -785,50 +782,50 @@
         <v>43846</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="140.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10">
+        <v>43853</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="E12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="G12" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>

</xml_diff>

<commit_message>
Add Jing Chen's fourth diary
</commit_message>
<xml_diff>
--- a/diaries/diary-JingChen.xlsx
+++ b/diaries/diary-JingChen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigAnnie\Desktop\winter2020\swe265-0121\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903C64D8-D1D1-443A-84C8-B3891F21FA0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DECA52-3C21-4E1E-B345-29911A182246}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="11136" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Achievements</t>
   </si>
   <si>
-    <t>Etc.</t>
-  </si>
-  <si>
     <t>Jing Chen</t>
   </si>
   <si>
@@ -126,7 +123,22 @@
     <t>Rafael Oliveira; Dongxin Xiang, Guowei Li</t>
   </si>
   <si>
-    <t>Know about usage of mental model, and how to improve mental model using UML by practice with examples.. After class, I did homework with my partners, which also help me understand what I have learned in class.</t>
+    <t>Guowei Li, Dongxin Xiang</t>
+  </si>
+  <si>
+    <t>Key expert practices, Structural vs behavioral models &amp; details in UML diagrams</t>
+  </si>
+  <si>
+    <t>Get used to the class and our professor's teaching style better than before.</t>
+  </si>
+  <si>
+    <t>Knew about usage of mental model, and how to improve mental model using UML by practice with examples.. After class, I did homework with my partners, which also help me understand what I have learned in class.</t>
+  </si>
+  <si>
+    <t>Understood the key expert practices and structural vs behavioral models. And gained details in UML diagrams</t>
+  </si>
+  <si>
+    <t>I feel three key expert practices are important during my practice. Statechart diagram is similar to FSM which I learnt from another course. I am glad to connect knowledge in different courses, which can further my understanding about it.</t>
   </si>
 </sst>
 </file>
@@ -632,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,7 +690,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -693,7 +705,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -708,7 +720,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -761,20 +773,20 @@
         <v>43839</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="G10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
@@ -782,22 +794,22 @@
         <v>43846</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="140.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -805,34 +817,46 @@
         <v>43853</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="E12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="10">
+        <v>43860</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
+      <c r="E13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>

</xml_diff>

<commit_message>
Add Jing Chen's fifth diary
</commit_message>
<xml_diff>
--- a/diaries/diary-JingChen.xlsx
+++ b/diaries/diary-JingChen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigAnnie\Desktop\winter2020\swe265-0121\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DECA52-3C21-4E1E-B345-29911A182246}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E996A63-3C94-4DAA-891D-62842D3CE33F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>I feel three key expert practices are important during my practice. Statechart diagram is similar to FSM which I learnt from another course. I am glad to connect knowledge in different courses, which can further my understanding about it.</t>
+  </si>
+  <si>
+    <t>Another three Key expert practices &amp; mental simulation &amp; practice</t>
+  </si>
+  <si>
+    <t>Understood the three key expert practices and how to use mental simulation to find our how does some code work. And did some practice about it.</t>
+  </si>
+  <si>
+    <t>I am glad to learn more skills that are useful in real life projects.</t>
+  </si>
+  <si>
+    <t>The three key expert are pretty useful. And indeed mental simulation should be combined with externalization and running the code (print) to work well. Mental simulation is easier to be undertood than mental model. The reason may be that we have learned about the JPacman project in other practice through other methods, where we solved other import frequent questions. So maybe the import frequent questions should be solved in an order like this in a project, if we need to know all the answers to all the questions. But still I will keep in mind, goal-driven is most efficient.</t>
   </si>
 </sst>
 </file>
@@ -644,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -858,14 +870,28 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+    <row r="14" spans="1:7" ht="263.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="10">
+        <v>43867</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>

</xml_diff>

<commit_message>
Add Jing Chen's sixth and seventh diary (#371)
Co-authored-by: scipanda <scipanda@qq.com>
</commit_message>
<xml_diff>
--- a/diaries/diary-JingChen.xlsx
+++ b/diaries/diary-JingChen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigAnnie\Desktop\winter2020\swe265-0121\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E996A63-3C94-4DAA-891D-62842D3CE33F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FB6CE1-9956-4106-8B69-FF6540E724C9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -151,6 +151,36 @@
   </si>
   <si>
     <t>The three key expert are pretty useful. And indeed mental simulation should be combined with externalization and running the code (print) to work well. Mental simulation is easier to be undertood than mental model. The reason may be that we have learned about the JPacman project in other practice through other methods, where we solved other import frequent questions. So maybe the import frequent questions should be solved in an order like this in a project, if we need to know all the answers to all the questions. But still I will keep in mind, goal-driven is most efficient.</t>
+  </si>
+  <si>
+    <t>Modify hw2 and complete hw3</t>
+  </si>
+  <si>
+    <t>Another three Key expert practices &amp; Big picture of development</t>
+  </si>
+  <si>
+    <t>Figure out how to improve hw2 with talking with Kaj. And we learned how to find "big picture" information about an open source project.</t>
+  </si>
+  <si>
+    <t>Gained knowledges about the three Key expert practices &amp; Big picture of development</t>
+  </si>
+  <si>
+    <t>I had a idea how to find info about an open source project and how people contribute to it.</t>
+  </si>
+  <si>
+    <t>Our group tried to figure out how to do the hw3. The requirement is simple, but we only learned the definations in class. So we need to figure out how and where to find related information.   And through teamwork, we get it done.</t>
+  </si>
+  <si>
+    <t>2/18/2020, 2/19/2020, 2/20/2020</t>
+  </si>
+  <si>
+    <t>14:30-17:00, 9:00-15:00 (2/20/2020)</t>
+  </si>
+  <si>
+    <t>Tired because of the midterm, since it was longder than I expected. And I did not do well in the next day's job interview since I was tired.  I wish I could handle the situation better. Glad to learn something useful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressured. I am still looking for an internship, and often have online assessments and interview during this quarter. As for me, it is not easy for these homework, since it took a lot of time. I have tried to make it balenced as possible as I can since I know both are important. But I feel more and more pressured recently. </t>
   </si>
 </sst>
 </file>
@@ -656,16 +686,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="34.6328125" customWidth="1"/>
+    <col min="1" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -676,7 +706,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -685,7 +715,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -694,7 +724,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -709,7 +739,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -724,7 +754,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -739,7 +769,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -748,7 +778,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -757,7 +787,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
@@ -780,7 +810,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>43839</v>
       </c>
@@ -801,7 +831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>43846</v>
       </c>
@@ -824,7 +854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="140.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="140.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>43853</v>
       </c>
@@ -847,7 +877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>43860</v>
       </c>
@@ -870,7 +900,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="263.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="280.8" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>43867</v>
       </c>
@@ -893,34 +923,62 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+    <row r="15" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>43874</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -929,7 +987,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -938,7 +996,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -947,7 +1005,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -956,7 +1014,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -965,7 +1023,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -974,7 +1032,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -983,7 +1041,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -992,7 +1050,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1001,7 +1059,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1010,7 +1068,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1019,7 +1077,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1028,7 +1086,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1037,7 +1095,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1046,7 +1104,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1055,7 +1113,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1064,7 +1122,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1073,7 +1131,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1082,7 +1140,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1091,7 +1149,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1100,7 +1158,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1109,7 +1167,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1118,7 +1176,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1127,7 +1185,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1136,7 +1194,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1145,7 +1203,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1154,7 +1212,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1163,7 +1221,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1172,7 +1230,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1181,7 +1239,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1190,7 +1248,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1199,7 +1257,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1208,7 +1266,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1217,7 +1275,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1226,7 +1284,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1235,7 +1293,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1244,7 +1302,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1253,7 +1311,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1262,7 +1320,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1271,7 +1329,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1280,7 +1338,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1289,7 +1347,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1298,7 +1356,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1307,7 +1365,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1316,7 +1374,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1325,7 +1383,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1334,7 +1392,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1343,7 +1401,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1352,7 +1410,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1361,7 +1419,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1370,7 +1428,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1379,7 +1437,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1388,7 +1446,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1397,7 +1455,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1406,7 +1464,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1415,7 +1473,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1424,7 +1482,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1433,7 +1491,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1442,7 +1500,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1451,7 +1509,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1460,7 +1518,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1469,7 +1527,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1478,7 +1536,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1487,7 +1545,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1496,7 +1554,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1505,7 +1563,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1514,7 +1572,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1523,7 +1581,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1532,7 +1590,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1541,7 +1599,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1550,7 +1608,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1559,7 +1617,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1568,7 +1626,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1577,7 +1635,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1586,7 +1644,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1595,7 +1653,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1604,7 +1662,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1613,7 +1671,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1622,7 +1680,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1631,7 +1689,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1640,7 +1698,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1649,7 +1707,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1658,7 +1716,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1667,7 +1725,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1676,7 +1734,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1685,7 +1743,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1694,7 +1752,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1703,7 +1761,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1712,7 +1770,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1721,7 +1779,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1730,7 +1788,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1739,7 +1797,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1748,7 +1806,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1757,7 +1815,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1766,7 +1824,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1775,7 +1833,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1784,7 +1842,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1793,7 +1851,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1802,7 +1860,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1811,7 +1869,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1820,7 +1878,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1829,7 +1887,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1838,7 +1896,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1847,7 +1905,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1856,7 +1914,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -1865,7 +1923,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -1874,7 +1932,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -1883,7 +1941,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>

</xml_diff>

<commit_message>
Add Jing Chen's wk8 Diaries
</commit_message>
<xml_diff>
--- a/diaries/diary-JingChen.xlsx
+++ b/diaries/diary-JingChen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigAnnie\Desktop\winter2020\swe265-w2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF48C371-8BED-4277-BB01-80EBEF2FE7E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76319A6F-1661-4869-A9D0-1C5F4CDAD18A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14040" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -208,6 +208,60 @@
   </si>
   <si>
     <t xml:space="preserve">Still a little confused about the definition of architure. I think it is because I have not gained enough experience in this field. Thank Sam and  Andre for helping us practice and stay on the right track. I plan to apply all the useful info I have learned to every one of my own projects in order to further understanding them. </t>
+  </si>
+  <si>
+    <t>20:00-21:00</t>
+  </si>
+  <si>
+    <t>17:00-20:00</t>
+  </si>
+  <si>
+    <t>Another three Key expert practices &amp; design patterns</t>
+  </si>
+  <si>
+    <t>Gained knowledges about the three Key expert practices &amp; some design patterns</t>
+  </si>
+  <si>
+    <t>Great guest talking. Good to know about someone who are excited to develope software for doing scientific research.</t>
+  </si>
+  <si>
+    <t>Useful skills and knowledge. Design patterns are popular currently and they are indeed important. I will learn more about them and try to use them in practice to improve my own project.</t>
+  </si>
+  <si>
+    <t>Look for five design patterns and open issues we can fix in our program. Record them.</t>
+  </si>
+  <si>
+    <t>Found five design patterns and several open issues we can fix in our program.</t>
+  </si>
+  <si>
+    <t>20:00-22:00</t>
+  </si>
+  <si>
+    <t>Some issues may be easier to be fixed than I expected</t>
+  </si>
+  <si>
+    <t>Not bad</t>
+  </si>
+  <si>
+    <t>Decide what design patterns to use for the assignment and open issues to fix in our program together. Discuss other related problems.</t>
+  </si>
+  <si>
+    <t>Decided five patterns to be used and two open issues to be fixed.</t>
+  </si>
+  <si>
+    <t>Review what we have done for the assignment and discuss what we should improve</t>
+  </si>
+  <si>
+    <t>We have completed the draft and filed all the problems we have not think through. We will go to find more information by ourselves, and then we will discuss again. And we plan to consult Kaj on Wednesday.</t>
+  </si>
+  <si>
+    <t>Made more things clear.</t>
+  </si>
+  <si>
+    <t>Design patterns in different levels have different usage, which makes them handy and popular.</t>
+  </si>
+  <si>
+    <t>Discussion is great</t>
   </si>
 </sst>
 </file>
@@ -710,16 +764,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="34.6640625" customWidth="1"/>
+    <col min="1" max="7" width="34.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -730,7 +784,7 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -739,7 +793,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -748,7 +802,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -763,7 +817,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -778,7 +832,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -793,7 +847,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -802,7 +856,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -811,7 +865,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
@@ -834,7 +888,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>43839</v>
       </c>
@@ -855,7 +909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>43846</v>
       </c>
@@ -878,7 +932,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="140.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="140.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>43853</v>
       </c>
@@ -901,7 +955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>43860</v>
       </c>
@@ -924,7 +978,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="280.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="263.5" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>43867</v>
       </c>
@@ -947,7 +1001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>43874</v>
       </c>
@@ -970,7 +1024,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>48</v>
       </c>
@@ -993,7 +1047,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>43881</v>
       </c>
@@ -1016,7 +1070,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>43884</v>
       </c>
@@ -1039,43 +1093,95 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
+    <row r="19" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="A19" s="9">
+        <v>43888</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="9">
+        <v>43889</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" s="9">
+        <v>43891</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="A22" s="9">
+        <v>43892</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1084,7 +1190,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1093,7 +1199,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1102,7 +1208,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1111,7 +1217,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1120,7 +1226,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1129,7 +1235,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1138,7 +1244,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1147,7 +1253,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1156,7 +1262,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1165,7 +1271,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1174,7 +1280,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1183,7 +1289,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1192,7 +1298,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1201,7 +1307,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1210,7 +1316,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1219,7 +1325,7 @@
       <c r="F38" s="6"/>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1228,7 +1334,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1237,7 +1343,7 @@
       <c r="F40" s="6"/>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1246,7 +1352,7 @@
       <c r="F41" s="6"/>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1255,7 +1361,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1264,7 +1370,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1273,7 +1379,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1282,7 +1388,7 @@
       <c r="F45" s="6"/>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1291,7 +1397,7 @@
       <c r="F46" s="6"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1300,7 +1406,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1309,7 +1415,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="7"/>
     </row>
-    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1318,7 +1424,7 @@
       <c r="F49" s="6"/>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -1327,7 +1433,7 @@
       <c r="F50" s="6"/>
       <c r="G50" s="7"/>
     </row>
-    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -1336,7 +1442,7 @@
       <c r="F51" s="6"/>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -1345,7 +1451,7 @@
       <c r="F52" s="6"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -1354,7 +1460,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="7"/>
     </row>
-    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1363,7 +1469,7 @@
       <c r="F54" s="6"/>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -1372,7 +1478,7 @@
       <c r="F55" s="6"/>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -1381,7 +1487,7 @@
       <c r="F56" s="6"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1390,7 +1496,7 @@
       <c r="F57" s="6"/>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1399,7 +1505,7 @@
       <c r="F58" s="6"/>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -1408,7 +1514,7 @@
       <c r="F59" s="6"/>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -1417,7 +1523,7 @@
       <c r="F60" s="6"/>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -1426,7 +1532,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -1435,7 +1541,7 @@
       <c r="F62" s="6"/>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -1444,7 +1550,7 @@
       <c r="F63" s="6"/>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -1453,7 +1559,7 @@
       <c r="F64" s="6"/>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -1462,7 +1568,7 @@
       <c r="F65" s="6"/>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -1471,7 +1577,7 @@
       <c r="F66" s="6"/>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -1480,7 +1586,7 @@
       <c r="F67" s="6"/>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -1489,7 +1595,7 @@
       <c r="F68" s="6"/>
       <c r="G68" s="7"/>
     </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -1498,7 +1604,7 @@
       <c r="F69" s="6"/>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -1507,7 +1613,7 @@
       <c r="F70" s="6"/>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -1516,7 +1622,7 @@
       <c r="F71" s="6"/>
       <c r="G71" s="7"/>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -1525,7 +1631,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="7"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -1534,7 +1640,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="7"/>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -1543,7 +1649,7 @@
       <c r="F74" s="6"/>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -1552,7 +1658,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -1561,7 +1667,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -1570,7 +1676,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="7"/>
     </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -1579,7 +1685,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -1588,7 +1694,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="7"/>
     </row>
-    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -1597,7 +1703,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -1606,7 +1712,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="7"/>
     </row>
-    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -1615,7 +1721,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="7"/>
     </row>
-    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -1624,7 +1730,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -1633,7 +1739,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="7"/>
     </row>
-    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -1642,7 +1748,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="7"/>
     </row>
-    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -1651,7 +1757,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="7"/>
     </row>
-    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -1660,7 +1766,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="7"/>
     </row>
-    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -1669,7 +1775,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="7"/>
     </row>
-    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -1678,7 +1784,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -1687,7 +1793,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -1696,7 +1802,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="7"/>
     </row>
-    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -1705,7 +1811,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="7"/>
     </row>
-    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -1714,7 +1820,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -1723,7 +1829,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -1732,7 +1838,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="7"/>
     </row>
-    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -1741,7 +1847,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -1750,7 +1856,7 @@
       <c r="F97" s="6"/>
       <c r="G97" s="7"/>
     </row>
-    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -1759,7 +1865,7 @@
       <c r="F98" s="6"/>
       <c r="G98" s="7"/>
     </row>
-    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
@@ -1768,7 +1874,7 @@
       <c r="F99" s="6"/>
       <c r="G99" s="7"/>
     </row>
-    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100" s="6"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
@@ -1777,7 +1883,7 @@
       <c r="F100" s="6"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
@@ -1786,7 +1892,7 @@
       <c r="F101" s="6"/>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
@@ -1795,7 +1901,7 @@
       <c r="F102" s="6"/>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
@@ -1804,7 +1910,7 @@
       <c r="F103" s="6"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
@@ -1813,7 +1919,7 @@
       <c r="F104" s="6"/>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
@@ -1822,7 +1928,7 @@
       <c r="F105" s="6"/>
       <c r="G105" s="7"/>
     </row>
-    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -1831,7 +1937,7 @@
       <c r="F106" s="6"/>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
@@ -1840,7 +1946,7 @@
       <c r="F107" s="6"/>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -1849,7 +1955,7 @@
       <c r="F108" s="6"/>
       <c r="G108" s="7"/>
     </row>
-    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -1858,7 +1964,7 @@
       <c r="F109" s="6"/>
       <c r="G109" s="7"/>
     </row>
-    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -1867,7 +1973,7 @@
       <c r="F110" s="6"/>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
@@ -1876,7 +1982,7 @@
       <c r="F111" s="6"/>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -1885,7 +1991,7 @@
       <c r="F112" s="6"/>
       <c r="G112" s="7"/>
     </row>
-    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -1894,7 +2000,7 @@
       <c r="F113" s="6"/>
       <c r="G113" s="7"/>
     </row>
-    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -1903,7 +2009,7 @@
       <c r="F114" s="6"/>
       <c r="G114" s="7"/>
     </row>
-    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -1912,7 +2018,7 @@
       <c r="F115" s="6"/>
       <c r="G115" s="7"/>
     </row>
-    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -1921,7 +2027,7 @@
       <c r="F116" s="6"/>
       <c r="G116" s="7"/>
     </row>
-    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -1930,7 +2036,7 @@
       <c r="F117" s="6"/>
       <c r="G117" s="7"/>
     </row>
-    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
@@ -1939,7 +2045,7 @@
       <c r="F118" s="6"/>
       <c r="G118" s="7"/>
     </row>
-    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
@@ -1948,7 +2054,7 @@
       <c r="F119" s="6"/>
       <c r="G119" s="7"/>
     </row>
-    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
@@ -1957,7 +2063,7 @@
       <c r="F120" s="6"/>
       <c r="G120" s="7"/>
     </row>
-    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
@@ -1966,7 +2072,7 @@
       <c r="F121" s="6"/>
       <c r="G121" s="7"/>
     </row>
-    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
@@ -1975,7 +2081,7 @@
       <c r="F122" s="6"/>
       <c r="G122" s="7"/>
     </row>
-    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="6"/>
@@ -1984,7 +2090,7 @@
       <c r="F123" s="6"/>
       <c r="G123" s="7"/>
     </row>
-    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
@@ -1993,7 +2099,7 @@
       <c r="F124" s="6"/>
       <c r="G124" s="7"/>
     </row>
-    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>

</xml_diff>

<commit_message>
Add Jing Chen's wk9 Diaries
</commit_message>
<xml_diff>
--- a/diaries/diary-JingChen.xlsx
+++ b/diaries/diary-JingChen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigAnnie\Desktop\winter2020\swe265-w2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76319A6F-1661-4869-A9D0-1C5F4CDAD18A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2262E2-6349-46B0-840E-7248AE7EF82B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -262,6 +262,33 @@
   </si>
   <si>
     <t>Discussion is great</t>
+  </si>
+  <si>
+    <t>19:50-20:00</t>
+  </si>
+  <si>
+    <t>Another three Key expert practices &amp; testing</t>
+  </si>
+  <si>
+    <t>Gained knowledges about the three Key expert practices, and got some idea how reading test cases can help us understand code by practice</t>
+  </si>
+  <si>
+    <t>When we write test cases, comments are still important to help us understand what is tested</t>
+  </si>
+  <si>
+    <t>Great guest talking. Good to learn in a happy way.</t>
+  </si>
+  <si>
+    <t>Think about and find information in our project about the last assignment.</t>
+  </si>
+  <si>
+    <t>Read some test cases in the project and got to learn more about it</t>
+  </si>
+  <si>
+    <t>Yesterday  It was great to know our proposed open issue was approved by Kaj. So we can continue working on it earlier.</t>
+  </si>
+  <si>
+    <t>When there are more test cases, it is easier to understand the code</t>
   </si>
 </sst>
 </file>
@@ -765,7 +792,7 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1181,23 +1208,47 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+    <row r="23" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+      <c r="A23" s="9">
+        <v>43895</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+      <c r="A24" s="9">
+        <v>43899</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7"/>
+      <c r="D24" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>

</xml_diff>

<commit_message>
Revised Jing Chen's wk9 diaries
</commit_message>
<xml_diff>
--- a/diaries/diary-JingChen.xlsx
+++ b/diaries/diary-JingChen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigAnnie\Desktop\winter2020\swe265-w2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigAnnie\Desktop\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2262E2-6349-46B0-840E-7248AE7EF82B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F541CC-8101-4BAA-8FC4-AB8F28BD581B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>When there are more test cases, it is easier to understand the code</t>
+  </si>
+  <si>
+    <t>Chunqi Zhao, Yijia Zhang, Thuc Nguyen</t>
   </si>
 </sst>
 </file>
@@ -792,7 +795,7 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1215,7 +1218,9 @@
       <c r="B23" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="D23" s="11" t="s">
         <v>80</v>
       </c>

</xml_diff>